<commit_message>
started to fix 2019 data
</commit_message>
<xml_diff>
--- a/Holidays/Skollov.xlsx
+++ b/Holidays/Skollov.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/svantepihl/Documents/R/CarFires/Holidays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F1B9BB-2208-E540-A795-E406CA13E20B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D756E02-3282-1F4E-9EF7-CB013D01E371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1026,10 +1026,10 @@
   <dimension ref="A1:M1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C176" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="I210" sqref="I210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>